<commit_message>
add roles to aoe_data sheet
</commit_message>
<xml_diff>
--- a/public/excel/aoe_data.xlsx
+++ b/public/excel/aoe_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="115">
   <si>
     <t>مدير الشئون الادارية</t>
   </si>
@@ -317,13 +317,55 @@
   </si>
   <si>
     <t>امير كليلة</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>abanob-mmdoh@aoe-egypt.com</t>
+  </si>
+  <si>
+    <t>ayzys-aamad@aoe-egypt.com</t>
+  </si>
+  <si>
+    <t>hlmy-kmal@aoe-egypt.com</t>
+  </si>
+  <si>
+    <t>nsr-syd@aoe-egypt.com</t>
+  </si>
+  <si>
+    <t>nbyl-odyd@aoe-egypt.com</t>
+  </si>
+  <si>
+    <t>nbyl-shokt@aoe-egypt.com</t>
+  </si>
+  <si>
+    <t>mhmod-khlf@aoe-egypt.com</t>
+  </si>
+  <si>
+    <t>aymn-aabd-alltyf@aoe-egypt.com</t>
+  </si>
+  <si>
+    <t>abrahym-mtoly@aoe-egypt.com</t>
+  </si>
+  <si>
+    <t>tomas-bshry@aoe-egypt.com</t>
+  </si>
+  <si>
+    <t>Secretary</t>
+  </si>
+  <si>
+    <t>Eng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,6 +388,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF636B6F"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -397,7 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -420,6 +468,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -723,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -740,7 +789,7 @@
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75">
+    <row r="1" spans="1:7" ht="18.75">
       <c r="A1" s="3" t="s">
         <v>42</v>
       </c>
@@ -759,8 +808,11 @@
       <c r="F1" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="18.75">
+      <c r="G1" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>100</v>
       </c>
@@ -779,8 +831,11 @@
       <c r="F2" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.75">
+      <c r="G2" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -799,8 +854,11 @@
       <c r="F3" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="18.75">
+      <c r="G3" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>50</v>
       </c>
@@ -819,8 +877,11 @@
       <c r="F4" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="18.75">
+      <c r="G4" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
@@ -830,15 +891,20 @@
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="8" t="s">
+        <v>103</v>
+      </c>
       <c r="E5" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="18.75">
+      <c r="G5" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -857,8 +923,11 @@
       <c r="F6" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="18.75">
+      <c r="G6" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
@@ -868,15 +937,20 @@
       <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="D7" s="8" t="s">
+        <v>40</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="18.75">
+      <c r="G7" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18.75">
       <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
@@ -886,15 +960,20 @@
       <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="8" t="s">
+        <v>104</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="18.75">
+      <c r="G8" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18.75">
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
@@ -913,8 +992,11 @@
       <c r="F9" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="18.75">
+      <c r="G9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18.75">
       <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
@@ -924,15 +1006,20 @@
       <c r="C10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="8" t="s">
+        <v>105</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="18.75">
+      <c r="G10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18.75">
       <c r="A11" s="1" t="s">
         <v>57</v>
       </c>
@@ -951,8 +1038,11 @@
       <c r="F11" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="18.75">
+      <c r="G11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18.75">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -971,8 +1061,11 @@
       <c r="F12" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="18.75">
+      <c r="G12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18.75">
       <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
@@ -991,8 +1084,11 @@
       <c r="F13" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="18.75">
+      <c r="G13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18.75">
       <c r="A14" s="1" t="s">
         <v>60</v>
       </c>
@@ -1011,8 +1107,11 @@
       <c r="F14" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="18.75">
+      <c r="G14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18.75">
       <c r="A15" s="1" t="s">
         <v>61</v>
       </c>
@@ -1031,8 +1130,11 @@
       <c r="F15" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="18.75">
+      <c r="G15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18.75">
       <c r="A16" s="1" t="s">
         <v>62</v>
       </c>
@@ -1042,15 +1144,20 @@
       <c r="C16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="5"/>
+      <c r="D16" s="8" t="s">
+        <v>106</v>
+      </c>
       <c r="E16" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="18.75">
+      <c r="G16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18.75">
       <c r="A17" s="1" t="s">
         <v>63</v>
       </c>
@@ -1060,15 +1167,20 @@
       <c r="C17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="5"/>
+      <c r="D17" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="E17" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="18.75">
+      <c r="G17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18.75">
       <c r="A18" s="1" t="s">
         <v>64</v>
       </c>
@@ -1078,15 +1190,20 @@
       <c r="C18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="5"/>
+      <c r="D18" s="8" t="s">
+        <v>108</v>
+      </c>
       <c r="E18" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="18.75">
+      <c r="G18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="18.75">
       <c r="A19" s="1" t="s">
         <v>65</v>
       </c>
@@ -1096,15 +1213,20 @@
       <c r="C19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="5"/>
+      <c r="D19" s="8" t="s">
+        <v>109</v>
+      </c>
       <c r="E19" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="18.75">
+      <c r="G19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="18.75">
       <c r="A20" s="1" t="s">
         <v>66</v>
       </c>
@@ -1114,15 +1236,20 @@
       <c r="C20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="7"/>
+      <c r="D20" s="8" t="s">
+        <v>110</v>
+      </c>
       <c r="E20" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="18.75">
+      <c r="G20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="18.75">
       <c r="A21" s="1" t="s">
         <v>67</v>
       </c>
@@ -1141,8 +1268,11 @@
       <c r="F21" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="18.75">
+      <c r="G21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="18.75">
       <c r="A22" s="1" t="s">
         <v>68</v>
       </c>
@@ -1161,8 +1291,11 @@
       <c r="F22" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="18.75">
+      <c r="G22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18.75">
       <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
@@ -1181,8 +1314,11 @@
       <c r="F23" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="18.75">
+      <c r="G23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="18.75">
       <c r="A24" s="1" t="s">
         <v>70</v>
       </c>
@@ -1192,15 +1328,20 @@
       <c r="C24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="5"/>
+      <c r="D24" s="8" t="s">
+        <v>111</v>
+      </c>
       <c r="E24" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="18.75">
+      <c r="G24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="18.75">
       <c r="A25" s="1" t="s">
         <v>98</v>
       </c>
@@ -1210,12 +1351,17 @@
       <c r="C25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="5"/>
+      <c r="D25" s="8" t="s">
+        <v>112</v>
+      </c>
       <c r="E25" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>94</v>
+      </c>
+      <c r="G25" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update aoe_data excel sheet
</commit_message>
<xml_diff>
--- a/public/excel/aoe_data.xlsx
+++ b/public/excel/aoe_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="116">
   <si>
     <t>مدير الشئون الادارية</t>
   </si>
@@ -359,6 +359,9 @@
   </si>
   <si>
     <t>Eng</t>
+  </si>
+  <si>
+    <t>krstyna-mnyr@aoe-egypt.com</t>
   </si>
 </sst>
 </file>
@@ -445,7 +448,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -469,6 +472,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -774,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -938,7 +942,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>47</v>
@@ -960,7 +964,7 @@
       <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="9" t="s">
         <v>104</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -1379,8 +1383,9 @@
     <hyperlink ref="D4" r:id="rId11"/>
     <hyperlink ref="D2" r:id="rId12"/>
     <hyperlink ref="D3" r:id="rId13"/>
+    <hyperlink ref="D8" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add two employees to aoe_ sheet and update jobtitle class
</commit_message>
<xml_diff>
--- a/public/excel/aoe_data.xlsx
+++ b/public/excel/aoe_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="126">
   <si>
     <t>مدير الشئون الادارية</t>
   </si>
@@ -367,13 +367,31 @@
     <t>مخازن</t>
   </si>
   <si>
-    <t>adel-thabet@aoe-egypt.com</t>
-  </si>
-  <si>
     <t>3dOgtjcgnK</t>
   </si>
   <si>
     <t>Maintenance Engineer</t>
+  </si>
+  <si>
+    <t>aoe@link. Net</t>
+  </si>
+  <si>
+    <t>ايمن جابر</t>
+  </si>
+  <si>
+    <t>محمد مصطفى</t>
+  </si>
+  <si>
+    <t>ayman_ghaber@aoe-egypt.com</t>
+  </si>
+  <si>
+    <t>mohamed_mostafa@aoe-egypt.com</t>
+  </si>
+  <si>
+    <t>asdu3IyeE</t>
+  </si>
+  <si>
+    <t>Aue83oww</t>
   </si>
 </sst>
 </file>
@@ -791,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1013,7 +1031,7 @@
         <v>78</v>
       </c>
       <c r="G9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75">
@@ -1036,7 +1054,7 @@
         <v>79</v>
       </c>
       <c r="G10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18.75">
@@ -1059,7 +1077,7 @@
         <v>80</v>
       </c>
       <c r="G11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18.75">
@@ -1082,7 +1100,7 @@
         <v>81</v>
       </c>
       <c r="G12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18.75">
@@ -1105,7 +1123,7 @@
         <v>82</v>
       </c>
       <c r="G13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75">
@@ -1128,7 +1146,7 @@
         <v>83</v>
       </c>
       <c r="G14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75">
@@ -1151,7 +1169,7 @@
         <v>84</v>
       </c>
       <c r="G15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75">
@@ -1164,7 +1182,7 @@
       <c r="C16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="9" t="s">
         <v>105</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -1174,7 +1192,7 @@
         <v>85</v>
       </c>
       <c r="G16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18.75">
@@ -1197,7 +1215,7 @@
         <v>86</v>
       </c>
       <c r="G17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18.75">
@@ -1220,7 +1238,7 @@
         <v>87</v>
       </c>
       <c r="G18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18.75">
@@ -1243,7 +1261,7 @@
         <v>88</v>
       </c>
       <c r="G19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18.75">
@@ -1266,7 +1284,7 @@
         <v>89</v>
       </c>
       <c r="G20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="18.75">
@@ -1289,7 +1307,7 @@
         <v>90</v>
       </c>
       <c r="G21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18.75">
@@ -1312,7 +1330,7 @@
         <v>91</v>
       </c>
       <c r="G22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18.75">
@@ -1335,7 +1353,7 @@
         <v>92</v>
       </c>
       <c r="G23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="18.75">
@@ -1358,7 +1376,7 @@
         <v>93</v>
       </c>
       <c r="G24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18.75">
@@ -1381,7 +1399,7 @@
         <v>94</v>
       </c>
       <c r="G25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1391,14 +1409,48 @@
       <c r="B26" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>118</v>
+    </row>
+    <row r="27" spans="1:7" ht="18.75">
+      <c r="A27" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="18.75">
+      <c r="A28" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1417,9 +1469,12 @@
     <hyperlink ref="D2" r:id="rId12"/>
     <hyperlink ref="D3" r:id="rId13"/>
     <hyperlink ref="D8" r:id="rId14"/>
-    <hyperlink ref="D26" r:id="rId15"/>
+    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D26" r:id="rId16"/>
+    <hyperlink ref="D27" r:id="rId17"/>
+    <hyperlink ref="D28" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>